<commit_message>
make attunits available for same time as defunits
</commit_message>
<xml_diff>
--- a/Einheitenbalancing.xlsx
+++ b/Einheitenbalancing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="24915" windowHeight="11790"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19440" windowHeight="11790" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Einheiten" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="83">
   <si>
     <t>Inra</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>Antigravitation</t>
+  </si>
+  <si>
+    <t>Plasmatechnik</t>
+  </si>
+  <si>
+    <t>Superkompression</t>
   </si>
 </sst>
 </file>
@@ -708,7 +714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1700,7 +1706,7 @@
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1752,10 +1758,10 @@
         <v>77</v>
       </c>
       <c r="K1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="L1" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="M1" t="s">
         <v>60</v>
@@ -2080,8 +2086,8 @@
       <c r="G8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="8">
-        <v>1</v>
+      <c r="H8" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>27</v>
@@ -2089,8 +2095,8 @@
       <c r="J8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>27</v>
+      <c r="K8" s="8">
+        <v>1</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>27</v>
@@ -2117,7 +2123,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>27</v>
@@ -2129,7 +2135,7 @@
         <v>27</v>
       </c>
       <c r="H9" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>27</v>
@@ -2137,8 +2143,8 @@
       <c r="J9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="8">
-        <v>1</v>
+      <c r="K9" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>27</v>
@@ -2525,7 +2531,7 @@
         <v>27</v>
       </c>
       <c r="O17" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -2572,7 +2578,7 @@
         <v>27</v>
       </c>
       <c r="O18" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -2619,7 +2625,7 @@
         <v>27</v>
       </c>
       <c r="O19" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -3071,8 +3077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3163,19 +3169,19 @@
         <v>54</v>
       </c>
       <c r="B5">
-        <v>30000</v>
+        <v>3000</v>
       </c>
       <c r="C5">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="D5">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="E5">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="F5" s="13">
-        <v>0.20833333333333334</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3183,44 +3189,44 @@
         <v>77</v>
       </c>
       <c r="B6">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="C6">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="D6">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="E6">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="F6" s="13">
-        <v>0.20833333333333334</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B7">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="C7">
-        <v>30000</v>
+        <v>3000</v>
       </c>
       <c r="D7">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="E7">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="F7" s="13">
-        <v>0.20833333333333334</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="B8">
         <v>35000</v>

</xml_diff>